<commit_message>
Nowe wyniki (do pracy), poprawki, czyszczenie projektu
</commit_message>
<xml_diff>
--- a/build_Windows/TestChiKwadrat.xlsx
+++ b/build_Windows/TestChiKwadrat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Kanjiklub\Documents\GitHub\CollisionDetectionComparison\build_Windows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3DB5CBE-2BA9-48E5-85CA-F448C1A791A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABAD444D-5777-474C-B891-ECB49EBABD27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{A3DFBAF8-C55C-4C09-AC04-CEAFEEF3C92E}"/>
+    <workbookView xWindow="-27840" yWindow="5745" windowWidth="25545" windowHeight="14025" activeTab="1" xr2:uid="{A3DFBAF8-C55C-4C09-AC04-CEAFEEF3C92E}"/>
   </bookViews>
   <sheets>
     <sheet name="AABB" sheetId="1" r:id="rId1"/>
@@ -695,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D072742-2FBC-4470-BC08-D326BB669599}">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1717,8 +1717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22AC8201-C491-418E-9356-2E604BF49263}">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1781,31 +1781,31 @@
       </c>
       <c r="D2" s="6">
         <f>(B2-$D$33)/$D$35</f>
-        <v>-3.741464913602587</v>
+        <v>-3.7865681982506421</v>
       </c>
       <c r="E2" s="6">
         <f>_xlfn.NORM.DIST(D2,0,1,1)</f>
-        <v>9.1475361191638489E-5</v>
+        <v>7.6371094332392217E-5</v>
       </c>
       <c r="F2" s="6">
         <f>E2</f>
-        <v>9.1475361191638489E-5</v>
+        <v>7.6371094332392217E-5</v>
       </c>
       <c r="G2" s="6">
         <f>F2*$C$13</f>
-        <v>6.8057668726579035E-2</v>
+        <v>5.659098090030263E-2</v>
       </c>
       <c r="H2" s="6">
         <f>C2-G2</f>
-        <v>-6.8057668726579035E-2</v>
+        <v>-5.659098090030263E-2</v>
       </c>
       <c r="I2" s="6">
         <f>H2^2</f>
-        <v>4.6318462724967736E-3</v>
+        <v>3.2025391192584173E-3</v>
       </c>
       <c r="J2" s="6">
         <f>I2/G2</f>
-        <v>6.8057668726579035E-2</v>
+        <v>5.6590980900302637E-2</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1820,31 +1820,31 @@
       </c>
       <c r="D3" s="6">
         <f t="shared" ref="D3:D12" si="0">(B3-$D$33)/$D$35</f>
-        <v>-2.9222624722487542</v>
+        <v>-2.9688945759560985</v>
       </c>
       <c r="E3" s="6">
         <f t="shared" ref="E3:E12" si="1">_xlfn.NORM.DIST(D3,0,1,1)</f>
-        <v>1.7374928107572634E-3</v>
+        <v>1.4943655759868026E-3</v>
       </c>
       <c r="F3" s="6">
         <f>E3-E2</f>
-        <v>1.6460174495656248E-3</v>
+        <v>1.4179944816544105E-3</v>
       </c>
       <c r="G3" s="6">
         <f t="shared" ref="G3:G12" si="2">F3*$C$13</f>
-        <v>1.2246369824768248</v>
+        <v>1.0507339109059182</v>
       </c>
       <c r="H3" s="6">
         <f t="shared" ref="H3:H12" si="3">C3-G3</f>
-        <v>-1.2246369824768248</v>
+        <v>-1.0507339109059182</v>
       </c>
       <c r="I3" s="6">
         <f t="shared" ref="I3:I12" si="4">H3^2</f>
-        <v>1.499735738849943</v>
+        <v>1.1040417515276459</v>
       </c>
       <c r="J3" s="6">
         <f t="shared" ref="J3:J12" si="5">I3/G3</f>
-        <v>1.2246369824768248</v>
+        <v>1.0507339109059182</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1855,35 +1855,35 @@
         <v>-2.5</v>
       </c>
       <c r="C4" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D4" s="6">
         <f t="shared" si="0"/>
-        <v>-2.103060030894921</v>
+        <v>-2.151220953661555</v>
       </c>
       <c r="E4" s="6">
         <f t="shared" si="1"/>
-        <v>1.7730261130233349E-2</v>
+        <v>1.572938195977322E-2</v>
       </c>
       <c r="F4" s="6">
         <f t="shared" ref="F4:F12" si="6">E4-E3</f>
-        <v>1.5992768319476085E-2</v>
+        <v>1.4235016383786417E-2</v>
       </c>
       <c r="G4" s="6">
         <f t="shared" si="2"/>
-        <v>11.898619629690208</v>
+        <v>10.548147140385735</v>
       </c>
       <c r="H4" s="6">
         <f t="shared" si="3"/>
-        <v>-6.8986196296902076</v>
+        <v>-3.5481471403857352</v>
       </c>
       <c r="I4" s="6">
         <f t="shared" si="4"/>
-        <v>47.590952795147054</v>
+        <v>12.589348129827471</v>
       </c>
       <c r="J4" s="6">
         <f t="shared" si="5"/>
-        <v>3.9997036863330786</v>
+        <v>1.1935127527399179</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1894,35 +1894,35 @@
         <v>-1.5</v>
       </c>
       <c r="C5" s="7">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" si="0"/>
-        <v>-1.2838575895410878</v>
+        <v>-1.3335473313670116</v>
       </c>
       <c r="E5" s="6">
         <f t="shared" si="1"/>
-        <v>9.9595894412083621E-2</v>
+        <v>9.1176126899420271E-2</v>
       </c>
       <c r="F5" s="6">
         <f t="shared" si="6"/>
-        <v>8.1865633281850272E-2</v>
+        <v>7.5446744939647051E-2</v>
       </c>
       <c r="G5" s="6">
         <f t="shared" si="2"/>
-        <v>60.908031161696606</v>
+        <v>55.906038000278464</v>
       </c>
       <c r="H5" s="6">
         <f t="shared" si="3"/>
-        <v>-3.9080311616966057</v>
+        <v>-11.906038000278464</v>
       </c>
       <c r="I5" s="6">
         <f t="shared" si="4"/>
-        <v>15.272707560791721</v>
+        <v>141.75374086407481</v>
       </c>
       <c r="J5" s="6">
         <f t="shared" si="5"/>
-        <v>0.25075030779186158</v>
+        <v>2.5355712179669885</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1937,31 +1937,31 @@
       </c>
       <c r="D6" s="6">
         <f t="shared" si="0"/>
-        <v>-0.46465514818725473</v>
+        <v>-0.51587370907246832</v>
       </c>
       <c r="E6" s="6">
         <f t="shared" si="1"/>
-        <v>0.32108921628936937</v>
+        <v>0.3029713087753142</v>
       </c>
       <c r="F6" s="6">
         <f t="shared" si="6"/>
-        <v>0.22149332187728576</v>
+        <v>0.21179518187589391</v>
       </c>
       <c r="G6" s="6">
         <f t="shared" si="2"/>
-        <v>164.7910314767006</v>
+        <v>156.94022977003738</v>
       </c>
       <c r="H6" s="6">
         <f t="shared" si="3"/>
-        <v>67.208968523299404</v>
+        <v>75.059770229962623</v>
       </c>
       <c r="I6" s="6">
         <f t="shared" si="4"/>
-        <v>4517.0454499658499</v>
+        <v>5633.9691069747832</v>
       </c>
       <c r="J6" s="6">
         <f t="shared" si="5"/>
-        <v>27.410748081909446</v>
+        <v>35.898820303947367</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1972,35 +1972,35 @@
         <v>0.5</v>
       </c>
       <c r="C7" s="7">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="D7" s="6">
         <f t="shared" si="0"/>
-        <v>0.35454729316657829</v>
+        <v>0.30179991322207506</v>
       </c>
       <c r="E7" s="6">
         <f t="shared" si="1"/>
-        <v>0.63853561603227016</v>
+        <v>0.61859770148698079</v>
       </c>
       <c r="F7" s="6">
         <f t="shared" si="6"/>
-        <v>0.31744639974290079</v>
+        <v>0.31562639271166659</v>
       </c>
       <c r="G7" s="6">
         <f t="shared" si="2"/>
-        <v>236.18012140871818</v>
+        <v>233.87915699934496</v>
       </c>
       <c r="H7" s="6">
         <f t="shared" si="3"/>
-        <v>-108.18012140871818</v>
+        <v>-123.87915699934496</v>
       </c>
       <c r="I7" s="6">
         <f t="shared" si="4"/>
-        <v>11702.938668005005</v>
+        <v>15346.045538868357</v>
       </c>
       <c r="J7" s="6">
         <f t="shared" si="5"/>
-        <v>49.550904615518633</v>
+        <v>65.615276434878453</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -2011,35 +2011,35 @@
         <v>1.5</v>
       </c>
       <c r="C8" s="7">
-        <v>242</v>
+        <v>270</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" si="0"/>
-        <v>1.1737497345204113</v>
+        <v>1.1194735355166185</v>
       </c>
       <c r="E8" s="6">
         <f t="shared" si="1"/>
-        <v>0.87975235854014078</v>
+        <v>0.86853091254671466</v>
       </c>
       <c r="F8" s="6">
         <f t="shared" si="6"/>
-        <v>0.24121674250787062</v>
+        <v>0.24993321105973387</v>
       </c>
       <c r="G8" s="6">
         <f t="shared" si="2"/>
-        <v>179.46525642585573</v>
+        <v>185.2005093952628</v>
       </c>
       <c r="H8" s="6">
         <f t="shared" si="3"/>
-        <v>62.534743574144272</v>
+        <v>84.799490604737201</v>
       </c>
       <c r="I8" s="6">
         <f t="shared" si="4"/>
-        <v>3910.5941538839784</v>
+        <v>7190.9536068229127</v>
       </c>
       <c r="J8" s="6">
         <f t="shared" si="5"/>
-        <v>21.790257522628629</v>
+        <v>38.827936436587621</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -2050,35 +2050,35 @@
         <v>2.5</v>
       </c>
       <c r="C9" s="7">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D9" s="6">
         <f t="shared" si="0"/>
-        <v>1.9929521758742443</v>
+        <v>1.9371471578111621</v>
       </c>
       <c r="E9" s="6">
         <f t="shared" si="1"/>
-        <v>0.97686665792402683</v>
+        <v>0.97363632125834543</v>
       </c>
       <c r="F9" s="6">
         <f t="shared" si="6"/>
-        <v>9.7114299383886049E-2</v>
+        <v>0.10510540871163077</v>
       </c>
       <c r="G9" s="6">
         <f t="shared" si="2"/>
-        <v>72.253038741611221</v>
+        <v>77.8831078553184</v>
       </c>
       <c r="H9" s="6">
         <f t="shared" si="3"/>
-        <v>-1.2530387416112205</v>
+        <v>-8.8831078553184</v>
       </c>
       <c r="I9" s="6">
         <f t="shared" si="4"/>
-        <v>1.570106087978631</v>
+        <v>78.909605169219461</v>
       </c>
       <c r="J9" s="6">
         <f t="shared" si="5"/>
-        <v>2.1730658188558537E-2</v>
+        <v>1.0131799737089069</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>30</v>
@@ -2095,35 +2095,35 @@
         <v>3.5</v>
       </c>
       <c r="C10" s="7">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D10" s="6">
         <f t="shared" si="0"/>
-        <v>2.8121546172280771</v>
+        <v>2.7548207801057054</v>
       </c>
       <c r="E10" s="6">
         <f t="shared" si="1"/>
-        <v>0.99753945791800713</v>
+        <v>0.99706378535808371</v>
       </c>
       <c r="F10" s="6">
         <f t="shared" si="6"/>
-        <v>2.0672799993980306E-2</v>
+        <v>2.3427464099738282E-2</v>
       </c>
       <c r="G10" s="6">
         <f t="shared" si="2"/>
-        <v>15.380563195521347</v>
+        <v>17.359750897906068</v>
       </c>
       <c r="H10" s="6">
         <f t="shared" si="3"/>
-        <v>-6.3805631955213471</v>
+        <v>-10.359750897906068</v>
       </c>
       <c r="I10" s="6">
         <f t="shared" si="4"/>
-        <v>40.711586692041585</v>
+        <v>107.32443866666557</v>
       </c>
       <c r="J10" s="6">
         <f t="shared" si="5"/>
-        <v>2.6469503212922891</v>
+        <v>6.1823720454197897</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>31</v>
@@ -2140,35 +2140,35 @@
         <v>4.5</v>
       </c>
       <c r="C11" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="6">
         <f t="shared" si="0"/>
-        <v>3.6313570585819104</v>
+        <v>3.5724944024002485</v>
       </c>
       <c r="E11" s="6">
         <f t="shared" si="1"/>
-        <v>0.99985903260055176</v>
+        <v>0.99982320147818871</v>
       </c>
       <c r="F11" s="6">
         <f t="shared" si="6"/>
-        <v>2.3195746825446228E-3</v>
+        <v>2.759416120104996E-3</v>
       </c>
       <c r="G11" s="6">
         <f t="shared" si="2"/>
-        <v>1.7257635638131994</v>
+        <v>2.0447273449978018</v>
       </c>
       <c r="H11" s="6">
         <f t="shared" si="3"/>
-        <v>-1.7257635638131994</v>
+        <v>-1.0447273449978018</v>
       </c>
       <c r="I11" s="6">
         <f t="shared" si="4"/>
-        <v>2.9782598781852347</v>
+        <v>1.091455225386156</v>
       </c>
       <c r="J11" s="6">
         <f t="shared" si="5"/>
-        <v>1.7257635638131994</v>
+        <v>0.53379010558854212</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>32</v>
@@ -2186,35 +2186,35 @@
         <v>5.5</v>
       </c>
       <c r="C12" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="6">
         <f t="shared" si="0"/>
-        <v>4.4505594999357436</v>
+        <v>4.3901680246947921</v>
       </c>
       <c r="E12" s="6">
         <f t="shared" si="1"/>
-        <v>0.99999571765702544</v>
+        <v>0.99999433684459438</v>
       </c>
       <c r="F12" s="6">
         <f t="shared" si="6"/>
-        <v>1.3668505647368434E-4</v>
+        <v>1.7113536640567251E-4</v>
       </c>
       <c r="G12" s="6">
         <f t="shared" si="2"/>
-        <v>0.10169368201642115</v>
+        <v>0.12681130650660333</v>
       </c>
       <c r="H12" s="6">
         <f t="shared" si="3"/>
-        <v>-0.10169368201642115</v>
+        <v>0.87318869349339667</v>
       </c>
       <c r="I12" s="6">
         <f t="shared" si="4"/>
-        <v>1.0341604962056978E-2</v>
+        <v>0.76245849444470504</v>
       </c>
       <c r="J12" s="6">
         <f t="shared" si="5"/>
-        <v>0.10169368201642115</v>
+        <v>6.0125434825088115</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>33</v>
@@ -2227,23 +2227,23 @@
       <c r="B13" s="12"/>
       <c r="C13" s="15">
         <f>SUM(C2:C12)</f>
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="12"/>
       <c r="F13" s="16">
         <f>SUM(F2:F12)</f>
-        <v>0.99999571765702544</v>
+        <v>0.99999433684459438</v>
       </c>
       <c r="G13" s="16">
         <f>SUM(G2:G12)</f>
-        <v>743.99681393682692</v>
+        <v>740.9958036018445</v>
       </c>
       <c r="H13" s="14"/>
       <c r="I13" s="12"/>
       <c r="J13" s="17">
         <f>SUM(J2:J12)</f>
-        <v>108.79119709069552</v>
+        <v>158.92032764515261</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>34</v>
@@ -2324,11 +2324,11 @@
       </c>
       <c r="E18" s="6">
         <f>B18-$D$33</f>
-        <v>-5.067204301075269</v>
+        <v>-5.1309041835357627</v>
       </c>
       <c r="F18" s="6">
         <f>E18^2</f>
-        <v>25.676559428835706</v>
+        <v>26.326177740624793</v>
       </c>
       <c r="G18" s="6">
         <f>F18*C18</f>
@@ -2353,11 +2353,11 @@
       </c>
       <c r="E19" s="6">
         <f t="shared" ref="E19:E28" si="10">B19-$D$33</f>
-        <v>-4.067204301075269</v>
+        <v>-4.1309041835357627</v>
       </c>
       <c r="F19" s="6">
         <f t="shared" ref="F19:F28" si="11">E19^2</f>
-        <v>16.542150826685166</v>
+        <v>17.064369373553266</v>
       </c>
       <c r="G19" s="6">
         <f t="shared" ref="G19:G28" si="12">F19*C19</f>
@@ -2374,23 +2374,23 @@
       </c>
       <c r="C20" s="7">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D20" s="6">
         <f t="shared" si="9"/>
-        <v>-15</v>
+        <v>-21</v>
       </c>
       <c r="E20" s="6">
         <f t="shared" si="10"/>
-        <v>-3.067204301075269</v>
+        <v>-3.1309041835357623</v>
       </c>
       <c r="F20" s="6">
         <f t="shared" si="11"/>
-        <v>9.4077422245346298</v>
+        <v>9.8025610064817386</v>
       </c>
       <c r="G20" s="6">
         <f t="shared" si="12"/>
-        <v>47.038711122673149</v>
+        <v>68.61792704537217</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="1"/>
@@ -2403,23 +2403,23 @@
       </c>
       <c r="C21" s="7">
         <f t="shared" si="8"/>
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D21" s="6">
         <f t="shared" si="9"/>
-        <v>-114</v>
+        <v>-88</v>
       </c>
       <c r="E21" s="6">
         <f t="shared" si="10"/>
-        <v>-2.067204301075269</v>
+        <v>-2.1309041835357623</v>
       </c>
       <c r="F21" s="6">
         <f t="shared" si="11"/>
-        <v>4.273333622384091</v>
+        <v>4.540752639410214</v>
       </c>
       <c r="G21" s="6">
         <f t="shared" si="12"/>
-        <v>243.58001647589319</v>
+        <v>199.79311613404943</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="1"/>
@@ -2440,15 +2440,15 @@
       </c>
       <c r="E22" s="6">
         <f t="shared" si="10"/>
-        <v>-1.0672043010752688</v>
+        <v>-1.1309041835357625</v>
       </c>
       <c r="F22" s="6">
         <f t="shared" si="11"/>
-        <v>1.1389250202335528</v>
+        <v>1.2789442723386897</v>
       </c>
       <c r="G22" s="6">
         <f t="shared" si="12"/>
-        <v>264.23060469418425</v>
+        <v>296.71507118257603</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="1"/>
@@ -2461,7 +2461,7 @@
       </c>
       <c r="C23" s="7">
         <f t="shared" si="8"/>
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="D23" s="6">
         <f t="shared" si="9"/>
@@ -2469,15 +2469,15 @@
       </c>
       <c r="E23" s="6">
         <f t="shared" si="10"/>
-        <v>-6.7204301075268813E-2</v>
+        <v>-0.13090418353576247</v>
       </c>
       <c r="F23" s="6">
         <f t="shared" si="11"/>
-        <v>4.516418083015377E-3</v>
+        <v>1.7135905267164585E-2</v>
       </c>
       <c r="G23" s="6">
         <f t="shared" si="12"/>
-        <v>0.57810151462596826</v>
+        <v>1.8849495793881044</v>
       </c>
       <c r="H23" s="8"/>
       <c r="I23" s="1"/>
@@ -2490,23 +2490,23 @@
       </c>
       <c r="C24" s="7">
         <f t="shared" si="8"/>
-        <v>242</v>
+        <v>270</v>
       </c>
       <c r="D24" s="6">
         <f t="shared" si="9"/>
-        <v>242</v>
+        <v>270</v>
       </c>
       <c r="E24" s="6">
         <f t="shared" si="10"/>
-        <v>0.93279569892473124</v>
+        <v>0.8690958164642375</v>
       </c>
       <c r="F24" s="6">
         <f t="shared" si="11"/>
-        <v>0.87010781593247788</v>
+        <v>0.75532753819563958</v>
       </c>
       <c r="G24" s="6">
         <f t="shared" si="12"/>
-        <v>210.56609145565966</v>
+        <v>203.93843531282269</v>
       </c>
       <c r="H24" s="8"/>
       <c r="I24" s="1"/>
@@ -2519,23 +2519,23 @@
       </c>
       <c r="C25" s="7">
         <f t="shared" si="8"/>
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D25" s="6">
         <f t="shared" si="9"/>
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E25" s="6">
         <f t="shared" si="10"/>
-        <v>1.9327956989247312</v>
+        <v>1.8690958164642375</v>
       </c>
       <c r="F25" s="6">
         <f t="shared" si="11"/>
-        <v>3.7356992137819405</v>
+        <v>3.4935191711241145</v>
       </c>
       <c r="G25" s="6">
         <f t="shared" si="12"/>
-        <v>265.23464417851778</v>
+        <v>241.0528228075639</v>
       </c>
       <c r="H25" s="8"/>
       <c r="I25" s="1"/>
@@ -2548,23 +2548,23 @@
       </c>
       <c r="C26" s="7">
         <f t="shared" si="8"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D26" s="6">
         <f t="shared" si="9"/>
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E26" s="6">
         <f t="shared" si="10"/>
-        <v>2.932795698924731</v>
+        <v>2.8690958164642377</v>
       </c>
       <c r="F26" s="6">
         <f t="shared" si="11"/>
-        <v>8.6012906116314021</v>
+        <v>8.2317108040525913</v>
       </c>
       <c r="G26" s="6">
         <f t="shared" si="12"/>
-        <v>77.411615504682615</v>
+        <v>57.621975628368141</v>
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="1"/>
@@ -2577,23 +2577,23 @@
       </c>
       <c r="C27" s="7">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" s="6">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E27" s="6">
         <f t="shared" si="10"/>
-        <v>3.932795698924731</v>
+        <v>3.8690958164642377</v>
       </c>
       <c r="F27" s="6">
         <f t="shared" si="11"/>
-        <v>15.466882009480864</v>
+        <v>14.969902436981066</v>
       </c>
       <c r="G27" s="6">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>14.969902436981066</v>
       </c>
       <c r="H27" s="8"/>
       <c r="I27" s="1"/>
@@ -2606,23 +2606,23 @@
       </c>
       <c r="C28" s="7">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" s="6">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E28" s="6">
         <f t="shared" si="10"/>
-        <v>4.932795698924731</v>
+        <v>4.8690958164642373</v>
       </c>
       <c r="F28" s="6">
         <f t="shared" si="11"/>
-        <v>24.332473407330326</v>
+        <v>23.708094069909539</v>
       </c>
       <c r="G28" s="6">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>23.708094069909539</v>
       </c>
       <c r="H28" s="8"/>
       <c r="I28" s="1"/>
@@ -2632,17 +2632,17 @@
       <c r="B29" s="12"/>
       <c r="C29" s="5">
         <f>SUM(C18:C28)</f>
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="D29" s="5">
         <f>SUM(D18:D28)</f>
-        <v>50</v>
+        <v>97</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="12"/>
       <c r="G29" s="5">
         <f>SUM(G18:G28)</f>
-        <v>1108.6397849462367</v>
+        <v>1108.3022941970312</v>
       </c>
       <c r="H29" s="8"/>
       <c r="I29" s="1"/>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="D33" s="6">
         <f>D29/C29</f>
-        <v>6.7204301075268813E-2</v>
+        <v>0.13090418353576247</v>
       </c>
       <c r="E33" s="11"/>
       <c r="F33" s="1"/>
@@ -2704,7 +2704,7 @@
       </c>
       <c r="D34" s="6">
         <f>G29/C29</f>
-        <v>1.4901072378309632</v>
+        <v>1.4956846075533485</v>
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="1"/>
@@ -2720,7 +2720,7 @@
       </c>
       <c r="D35" s="6">
         <f>SQRT(D34)</f>
-        <v>1.2206994871101418</v>
+        <v>1.2229818508683392</v>
       </c>
       <c r="E35" s="11"/>
       <c r="F35" s="1"/>
@@ -2738,8 +2738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19CD015E-35D1-4646-BA16-39A53C5518A6}">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2802,31 +2802,31 @@
       </c>
       <c r="D2" s="6">
         <f>(B2-$D$33)/$D$35</f>
-        <v>-4.1539636713388637</v>
+        <v>-4.6374227913954016</v>
       </c>
       <c r="E2" s="6">
         <f>_xlfn.NORM.DIST(D2,0,1,1)</f>
-        <v>1.6338253809632177E-5</v>
+        <v>1.7639016147499319E-6</v>
       </c>
       <c r="F2" s="6">
         <f>E2</f>
-        <v>1.6338253809632177E-5</v>
+        <v>1.7639016147499319E-6</v>
       </c>
       <c r="G2" s="6">
         <f>F2*$C$13</f>
-        <v>8.3488476967220424E-3</v>
+        <v>1.7762489260531814E-3</v>
       </c>
       <c r="H2" s="6">
         <f>C2-G2</f>
-        <v>-8.3488476967220424E-3</v>
+        <v>-1.7762489260531814E-3</v>
       </c>
       <c r="I2" s="6">
         <f>H2^2</f>
-        <v>6.9703257863060948E-5</v>
+        <v>3.1550602473050805E-6</v>
       </c>
       <c r="J2" s="6">
         <f>I2/G2</f>
-        <v>8.3488476967220424E-3</v>
+        <v>1.7762489260531814E-3</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -2837,35 +2837,35 @@
         <v>-3.5</v>
       </c>
       <c r="C3" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="6">
         <f t="shared" ref="D3:D12" si="0">(B3-$D$33)/$D$35</f>
-        <v>-3.1993086517507554</v>
+        <v>-3.5802898540020416</v>
       </c>
       <c r="E3" s="6">
         <f t="shared" ref="E3:E12" si="1">_xlfn.NORM.DIST(D3,0,1,1)</f>
-        <v>6.8878799754094129E-4</v>
+        <v>1.716066374427067E-4</v>
       </c>
       <c r="F3" s="6">
         <f>E3-E2</f>
-        <v>6.7244974373130916E-4</v>
+        <v>1.6984273582795677E-4</v>
       </c>
       <c r="G3" s="6">
         <f t="shared" ref="G3:G12" si="2">F3*$C$13</f>
-        <v>0.34362181904669897</v>
+        <v>0.17103163497875246</v>
       </c>
       <c r="H3" s="6">
         <f t="shared" ref="H3:H12" si="3">C3-G3</f>
-        <v>0.65637818095330103</v>
+        <v>-0.17103163497875246</v>
       </c>
       <c r="I3" s="6">
         <f t="shared" ref="I3:I12" si="4">H3^2</f>
-        <v>0.43083231643156439</v>
+        <v>2.9251820163505221E-2</v>
       </c>
       <c r="J3" s="6">
         <f t="shared" ref="J3:J12" si="5">I3/G3</f>
-        <v>1.2537979038316345</v>
+        <v>0.17103163497875246</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -2876,35 +2876,35 @@
         <v>-2.5</v>
       </c>
       <c r="C4" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4" s="6">
         <f t="shared" si="0"/>
-        <v>-2.2446536321626467</v>
+        <v>-2.5231569166086811</v>
       </c>
       <c r="E4" s="6">
         <f t="shared" si="1"/>
-        <v>1.2395188437386016E-2</v>
+        <v>5.8153244617139927E-3</v>
       </c>
       <c r="F4" s="6">
         <f t="shared" ref="F4:F12" si="6">E4-E3</f>
-        <v>1.1706400439845074E-2</v>
+        <v>5.6437178242712861E-3</v>
       </c>
       <c r="G4" s="6">
         <f t="shared" si="2"/>
-        <v>5.9819706247608329</v>
+        <v>5.6832238490411848</v>
       </c>
       <c r="H4" s="6">
         <f t="shared" si="3"/>
-        <v>-1.9819706247608329</v>
+        <v>-0.68322384904118483</v>
       </c>
       <c r="I4" s="6">
         <f t="shared" si="4"/>
-        <v>3.9282075574148463</v>
+        <v>0.46679482789865173</v>
       </c>
       <c r="J4" s="6">
         <f t="shared" si="5"/>
-        <v>0.65667449805838873</v>
+        <v>8.2135569581234177E-2</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2915,35 +2915,35 @@
         <v>-1.5</v>
       </c>
       <c r="C5" s="7">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" si="0"/>
-        <v>-1.2899986125745382</v>
+        <v>-1.4660239792153207</v>
       </c>
       <c r="E5" s="6">
         <f t="shared" si="1"/>
-        <v>9.8525569910141109E-2</v>
+        <v>7.1320877144263953E-2</v>
       </c>
       <c r="F5" s="6">
         <f t="shared" si="6"/>
-        <v>8.6130381472755091E-2</v>
+        <v>6.5505552682549956E-2</v>
       </c>
       <c r="G5" s="6">
         <f t="shared" si="2"/>
-        <v>44.01262493257785</v>
+        <v>65.964091551327812</v>
       </c>
       <c r="H5" s="6">
         <f t="shared" si="3"/>
-        <v>-5.0126249325778502</v>
+        <v>-5.9640915513278117</v>
       </c>
       <c r="I5" s="6">
         <f t="shared" si="4"/>
-        <v>25.126408714701096</v>
+        <v>35.570388032619782</v>
       </c>
       <c r="J5" s="6">
         <f t="shared" si="5"/>
-        <v>0.57089093761600884</v>
+        <v>0.53923865539695703</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2954,35 +2954,35 @@
         <v>-0.5</v>
       </c>
       <c r="C6" s="7">
-        <v>141</v>
+        <v>262</v>
       </c>
       <c r="D6" s="6">
         <f t="shared" si="0"/>
-        <v>-0.33534359298642957</v>
+        <v>-0.40889104182196023</v>
       </c>
       <c r="E6" s="6">
         <f t="shared" si="1"/>
-        <v>0.36868295653597027</v>
+        <v>0.34130981169513042</v>
       </c>
       <c r="F6" s="6">
         <f t="shared" si="6"/>
-        <v>0.27015738662582917</v>
+        <v>0.26998893455086648</v>
       </c>
       <c r="G6" s="6">
         <f t="shared" si="2"/>
-        <v>138.05042456579869</v>
+        <v>271.87885709272257</v>
       </c>
       <c r="H6" s="6">
         <f t="shared" si="3"/>
-        <v>2.9495754342013072</v>
+        <v>-9.8788570927225692</v>
       </c>
       <c r="I6" s="6">
         <f t="shared" si="4"/>
-        <v>8.6999952420438298</v>
+        <v>97.591817458435017</v>
       </c>
       <c r="J6" s="6">
         <f t="shared" si="5"/>
-        <v>6.3020416412389729E-2</v>
+        <v>0.35895331656904805</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2993,35 +2993,35 @@
         <v>0.5</v>
       </c>
       <c r="C7" s="7">
-        <v>195</v>
+        <v>436</v>
       </c>
       <c r="D7" s="6">
         <f t="shared" si="0"/>
-        <v>0.61931142660167904</v>
+        <v>0.64824189557140033</v>
       </c>
       <c r="E7" s="6">
         <f t="shared" si="1"/>
-        <v>0.73214439083961125</v>
+        <v>0.74158574578469594</v>
       </c>
       <c r="F7" s="6">
         <f t="shared" si="6"/>
-        <v>0.36346143430364097</v>
+        <v>0.40027593408956552</v>
       </c>
       <c r="G7" s="6">
         <f t="shared" si="2"/>
-        <v>185.72879292916053</v>
+        <v>403.07786562819246</v>
       </c>
       <c r="H7" s="6">
         <f t="shared" si="3"/>
-        <v>9.2712070708394663</v>
+        <v>32.922134371807545</v>
       </c>
       <c r="I7" s="6">
         <f t="shared" si="4"/>
-        <v>85.955280550383719</v>
+        <v>1083.8669315953518</v>
       </c>
       <c r="J7" s="6">
         <f t="shared" si="5"/>
-        <v>0.46279997406308576</v>
+        <v>2.6889765576836053</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -3032,35 +3032,35 @@
         <v>1.5</v>
       </c>
       <c r="C8" s="7">
-        <v>107</v>
+        <v>208</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" si="0"/>
-        <v>1.5739664461897878</v>
+        <v>1.7053748329647609</v>
       </c>
       <c r="E8" s="6">
         <f t="shared" si="1"/>
-        <v>0.94225239657973348</v>
+        <v>0.9559377305008725</v>
       </c>
       <c r="F8" s="6">
         <f t="shared" si="6"/>
-        <v>0.21010800574012223</v>
+        <v>0.21435198471617656</v>
       </c>
       <c r="G8" s="6">
         <f t="shared" si="2"/>
-        <v>107.36519093320246</v>
+        <v>215.85244860918979</v>
       </c>
       <c r="H8" s="6">
         <f t="shared" si="3"/>
-        <v>-0.36519093320245588</v>
+        <v>-7.8524486091897927</v>
       </c>
       <c r="I8" s="6">
         <f t="shared" si="4"/>
-        <v>0.13336441769328058</v>
+        <v>61.660949159966712</v>
       </c>
       <c r="J8" s="6">
         <f t="shared" si="5"/>
-        <v>1.2421569461582163E-3</v>
+        <v>0.28566249564120783</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -3071,35 +3071,35 @@
         <v>2.5</v>
       </c>
       <c r="C9" s="7">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D9" s="6">
         <f t="shared" si="0"/>
-        <v>2.5286214657778965</v>
+        <v>2.7625077703581211</v>
       </c>
       <c r="E9" s="6">
         <f t="shared" si="1"/>
-        <v>0.99427442723757264</v>
+        <v>0.99713204017786927</v>
       </c>
       <c r="F9" s="6">
         <f t="shared" si="6"/>
-        <v>5.2022030657839169E-2</v>
+        <v>4.1194309676996776E-2</v>
       </c>
       <c r="G9" s="6">
         <f t="shared" si="2"/>
-        <v>26.583257666155816</v>
+        <v>41.482669844735753</v>
       </c>
       <c r="H9" s="6">
         <f t="shared" si="3"/>
-        <v>-6.5832576661558164</v>
+        <v>-8.4826698447357529</v>
       </c>
       <c r="I9" s="6">
         <f t="shared" si="4"/>
-        <v>43.339281498999327</v>
+        <v>71.955687694789276</v>
       </c>
       <c r="J9" s="6">
         <f t="shared" si="5"/>
-        <v>1.6303224399083436</v>
+        <v>1.7345963498518797</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>30</v>
@@ -3116,35 +3116,35 @@
         <v>3.5</v>
       </c>
       <c r="C10" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="6">
         <f t="shared" si="0"/>
-        <v>3.4832764853660052</v>
+        <v>3.819640707751482</v>
       </c>
       <c r="E10" s="6">
         <f t="shared" si="1"/>
-        <v>0.99975234173353045</v>
+        <v>0.99993317689797434</v>
       </c>
       <c r="F10" s="6">
         <f t="shared" si="6"/>
-        <v>5.477914495957803E-3</v>
+        <v>2.8011367201050685E-3</v>
       </c>
       <c r="G10" s="6">
         <f t="shared" si="2"/>
-        <v>2.7992143074344371</v>
+        <v>2.8207446771458038</v>
       </c>
       <c r="H10" s="6">
         <f t="shared" si="3"/>
-        <v>1.2007856925655629</v>
+        <v>0.17925532285419621</v>
       </c>
       <c r="I10" s="6">
         <f t="shared" si="4"/>
-        <v>1.4418862794701586</v>
+        <v>3.2132470771562116E-2</v>
       </c>
       <c r="J10" s="6">
         <f t="shared" si="5"/>
-        <v>0.51510392599832422</v>
+        <v>1.1391485032979182E-2</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>31</v>
@@ -3165,31 +3165,31 @@
       </c>
       <c r="D11" s="6">
         <f t="shared" si="0"/>
-        <v>4.4379315049541139</v>
+        <v>4.8767736451448425</v>
       </c>
       <c r="E11" s="6">
         <f t="shared" si="1"/>
-        <v>0.99999545862447192</v>
+        <v>0.99999946082471447</v>
       </c>
       <c r="F11" s="6">
         <f t="shared" si="6"/>
-        <v>2.4311689094147493E-4</v>
+        <v>6.6283926740129395E-5</v>
       </c>
       <c r="G11" s="6">
         <f t="shared" si="2"/>
-        <v>0.12423273127109369</v>
+        <v>6.6747914227310301E-2</v>
       </c>
       <c r="H11" s="6">
         <f t="shared" si="3"/>
-        <v>-0.12423273127109369</v>
+        <v>-6.6747914227310301E-2</v>
       </c>
       <c r="I11" s="6">
         <f t="shared" si="4"/>
-        <v>1.543377151907578E-2</v>
+        <v>4.4552840536963732E-3</v>
       </c>
       <c r="J11" s="6">
         <f t="shared" si="5"/>
-        <v>0.12423273127109369</v>
+        <v>6.6747914227310301E-2</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>32</v>
@@ -3211,31 +3211,31 @@
       </c>
       <c r="D12" s="6">
         <f t="shared" si="0"/>
-        <v>5.3925865245422226</v>
+        <v>5.9339065825382038</v>
       </c>
       <c r="E12" s="6">
         <f t="shared" si="1"/>
-        <v>0.99999996527468082</v>
+        <v>0.99999999852094912</v>
       </c>
       <c r="F12" s="6">
         <f t="shared" si="6"/>
-        <v>4.5066502089019522E-6</v>
+        <v>5.3769623464816618E-7</v>
       </c>
       <c r="G12" s="6">
         <f t="shared" si="2"/>
-        <v>2.3028982567488976E-3</v>
+        <v>5.4146010829070335E-4</v>
       </c>
       <c r="H12" s="6">
         <f t="shared" si="3"/>
-        <v>-2.3028982567488976E-3</v>
+        <v>-5.4146010829070335E-4</v>
       </c>
       <c r="I12" s="6">
         <f t="shared" si="4"/>
-        <v>5.3033403809371116E-6</v>
+        <v>2.9317904887018021E-7</v>
       </c>
       <c r="J12" s="6">
         <f t="shared" si="5"/>
-        <v>2.3028982567488976E-3</v>
+        <v>5.4146010829070335E-4</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>33</v>
@@ -3248,23 +3248,23 @@
       <c r="B13" s="12"/>
       <c r="C13" s="15">
         <f>SUM(C2:C12)</f>
-        <v>511</v>
+        <v>1007</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="12"/>
       <c r="F13" s="16">
         <f>SUM(F2:F12)</f>
-        <v>0.99999996527468082</v>
+        <v>0.99999999852094912</v>
       </c>
       <c r="G13" s="16">
         <f>SUM(G2:G12)</f>
-        <v>510.99998225536194</v>
+        <v>1006.9999985105958</v>
       </c>
       <c r="H13" s="14"/>
       <c r="I13" s="12"/>
       <c r="J13" s="17">
         <f>SUM(J2:J12)</f>
-        <v>5.2887367300588988</v>
+        <v>5.9410516879973176</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>34</v>
@@ -3345,11 +3345,11 @@
       </c>
       <c r="E18" s="6">
         <f>B18-$D$33</f>
-        <v>-4.8512720156555771</v>
+        <v>-4.8867924528301883</v>
       </c>
       <c r="F18" s="6">
         <f>E18^2</f>
-        <v>23.534840169882926</v>
+        <v>23.880740477038088</v>
       </c>
       <c r="G18" s="6">
         <f>F18*C18</f>
@@ -3366,23 +3366,23 @@
       </c>
       <c r="C19" s="7">
         <f t="shared" ref="C19:C28" si="8">C3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" s="6">
         <f t="shared" ref="D19:D28" si="9">C19*B19</f>
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="E19" s="6">
         <f t="shared" ref="E19:E28" si="10">B19-$D$33</f>
-        <v>-3.8512720156555771</v>
+        <v>-3.8867924528301887</v>
       </c>
       <c r="F19" s="6">
         <f t="shared" ref="F19:F28" si="11">E19^2</f>
-        <v>14.832296138571772</v>
+        <v>15.107155571377715</v>
       </c>
       <c r="G19" s="6">
         <f t="shared" ref="G19:G28" si="12">F19*C19</f>
-        <v>14.832296138571772</v>
+        <v>0</v>
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="1"/>
@@ -3395,23 +3395,23 @@
       </c>
       <c r="C20" s="7">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D20" s="6">
         <f t="shared" si="9"/>
-        <v>-12</v>
+        <v>-15</v>
       </c>
       <c r="E20" s="6">
         <f t="shared" si="10"/>
-        <v>-2.8512720156555771</v>
+        <v>-2.8867924528301887</v>
       </c>
       <c r="F20" s="6">
         <f t="shared" si="11"/>
-        <v>8.129752107260618</v>
+        <v>8.3335706657173372</v>
       </c>
       <c r="G20" s="6">
         <f t="shared" si="12"/>
-        <v>32.519008429042472</v>
+        <v>41.667853328586688</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="1"/>
@@ -3424,23 +3424,23 @@
       </c>
       <c r="C21" s="7">
         <f t="shared" si="8"/>
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="D21" s="6">
         <f t="shared" si="9"/>
-        <v>-78</v>
+        <v>-120</v>
       </c>
       <c r="E21" s="6">
         <f t="shared" si="10"/>
-        <v>-1.8512720156555773</v>
+        <v>-1.8867924528301887</v>
       </c>
       <c r="F21" s="6">
         <f t="shared" si="11"/>
-        <v>3.4272080759494639</v>
+        <v>3.5599857600569598</v>
       </c>
       <c r="G21" s="6">
         <f t="shared" si="12"/>
-        <v>133.6611149620291</v>
+        <v>213.59914560341758</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="1"/>
@@ -3453,23 +3453,23 @@
       </c>
       <c r="C22" s="7">
         <f t="shared" si="8"/>
-        <v>141</v>
+        <v>262</v>
       </c>
       <c r="D22" s="6">
         <f t="shared" si="9"/>
-        <v>-141</v>
+        <v>-262</v>
       </c>
       <c r="E22" s="6">
         <f t="shared" si="10"/>
-        <v>-0.85127201565557731</v>
+        <v>-0.8867924528301887</v>
       </c>
       <c r="F22" s="6">
         <f t="shared" si="11"/>
-        <v>0.72466404463830947</v>
+        <v>0.78640085439658247</v>
       </c>
       <c r="G22" s="6">
         <f t="shared" si="12"/>
-        <v>102.17763029400163</v>
+        <v>206.03702385190462</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="1"/>
@@ -3482,7 +3482,7 @@
       </c>
       <c r="C23" s="7">
         <f t="shared" si="8"/>
-        <v>195</v>
+        <v>436</v>
       </c>
       <c r="D23" s="6">
         <f t="shared" si="9"/>
@@ -3490,15 +3490,15 @@
       </c>
       <c r="E23" s="6">
         <f t="shared" si="10"/>
-        <v>0.14872798434442269</v>
+        <v>0.11320754716981132</v>
       </c>
       <c r="F23" s="6">
         <f t="shared" si="11"/>
-        <v>2.2120013327154842E-2</v>
+        <v>1.2815948736205056E-2</v>
       </c>
       <c r="G23" s="6">
         <f t="shared" si="12"/>
-        <v>4.3134025987951938</v>
+        <v>5.5877536489854043</v>
       </c>
       <c r="H23" s="8"/>
       <c r="I23" s="1"/>
@@ -3511,23 +3511,23 @@
       </c>
       <c r="C24" s="7">
         <f t="shared" si="8"/>
-        <v>107</v>
+        <v>208</v>
       </c>
       <c r="D24" s="6">
         <f t="shared" si="9"/>
-        <v>107</v>
+        <v>208</v>
       </c>
       <c r="E24" s="6">
         <f t="shared" si="10"/>
-        <v>1.1487279843444227</v>
+        <v>1.1132075471698113</v>
       </c>
       <c r="F24" s="6">
         <f t="shared" si="11"/>
-        <v>1.3195759820160002</v>
+        <v>1.2392310430758275</v>
       </c>
       <c r="G24" s="6">
         <f t="shared" si="12"/>
-        <v>141.19463007571201</v>
+        <v>257.7600569597721</v>
       </c>
       <c r="H24" s="8"/>
       <c r="I24" s="1"/>
@@ -3540,23 +3540,23 @@
       </c>
       <c r="C25" s="7">
         <f t="shared" si="8"/>
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D25" s="6">
         <f t="shared" si="9"/>
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="E25" s="6">
         <f t="shared" si="10"/>
-        <v>2.1487279843444229</v>
+        <v>2.1132075471698113</v>
       </c>
       <c r="F25" s="6">
         <f t="shared" si="11"/>
-        <v>4.6170319507048463</v>
+        <v>4.4656461374154501</v>
       </c>
       <c r="G25" s="6">
         <f t="shared" si="12"/>
-        <v>92.340639014096922</v>
+        <v>147.36632253470987</v>
       </c>
       <c r="H25" s="8"/>
       <c r="I25" s="1"/>
@@ -3569,23 +3569,23 @@
       </c>
       <c r="C26" s="7">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D26" s="6">
         <f t="shared" si="9"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E26" s="6">
         <f t="shared" si="10"/>
-        <v>3.1487279843444229</v>
+        <v>3.1132075471698113</v>
       </c>
       <c r="F26" s="6">
         <f t="shared" si="11"/>
-        <v>9.914487919393693</v>
+        <v>9.6920612317550727</v>
       </c>
       <c r="G26" s="6">
         <f t="shared" si="12"/>
-        <v>39.657951677574772</v>
+        <v>29.076183695265218</v>
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="1"/>
@@ -3606,11 +3606,11 @@
       </c>
       <c r="E27" s="6">
         <f t="shared" si="10"/>
-        <v>4.1487279843444229</v>
+        <v>4.1132075471698117</v>
       </c>
       <c r="F27" s="6">
         <f t="shared" si="11"/>
-        <v>17.211943888082537</v>
+        <v>16.918476326094698</v>
       </c>
       <c r="G27" s="6">
         <f t="shared" si="12"/>
@@ -3635,11 +3635,11 @@
       </c>
       <c r="E28" s="6">
         <f t="shared" si="10"/>
-        <v>5.1487279843444229</v>
+        <v>5.1132075471698117</v>
       </c>
       <c r="F28" s="6">
         <f t="shared" si="11"/>
-        <v>26.509399856771385</v>
+        <v>26.144891420434323</v>
       </c>
       <c r="G28" s="6">
         <f t="shared" si="12"/>
@@ -3653,17 +3653,17 @@
       <c r="B29" s="12"/>
       <c r="C29" s="5">
         <f>SUM(C18:C28)</f>
-        <v>511</v>
+        <v>1007</v>
       </c>
       <c r="D29" s="5">
         <f>SUM(D18:D28)</f>
-        <v>-76</v>
+        <v>-114</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="12"/>
       <c r="G29" s="5">
         <f>SUM(G18:G28)</f>
-        <v>560.69667318982397</v>
+        <v>901.09433962264143</v>
       </c>
       <c r="H29" s="8"/>
       <c r="I29" s="1"/>
@@ -3709,7 +3709,7 @@
       </c>
       <c r="D33" s="6">
         <f>D29/C29</f>
-        <v>-0.14872798434442269</v>
+        <v>-0.11320754716981132</v>
       </c>
       <c r="E33" s="11"/>
       <c r="F33" s="1"/>
@@ -3725,7 +3725,7 @@
       </c>
       <c r="D34" s="6">
         <f>G29/C29</f>
-        <v>1.0972537635808688</v>
+        <v>0.89483052594105406</v>
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="1"/>
@@ -3741,7 +3741,7 @@
       </c>
       <c r="D35" s="6">
         <f>SQRT(D34)</f>
-        <v>1.0474988131644201</v>
+        <v>0.94595482235731221</v>
       </c>
       <c r="E35" s="11"/>
       <c r="F35" s="1"/>

</xml_diff>